<commit_message>
Removed unecessary files, and created a folder with the original raw data
</commit_message>
<xml_diff>
--- a/merged_data.xlsx
+++ b/merged_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/k/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielcanuto/Documents/Courses/STAT205/Project 1/STAT-205/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3149F1BA-E099-844E-8C9B-45553F0DF692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1AB356-736B-5145-9D5D-A9221A1828EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -83,10 +83,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:D823"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>